<commit_message>
Author        : Priyanka Chaudhary Description   : Excel to get offline status with Logged time for Pooja, Priyanka, Prateek File Added    : WorkPlan-BUGFIXING.xlsx
</commit_message>
<xml_diff>
--- a/Requirements/WorkPlan-BUGFIXING.xlsx
+++ b/Requirements/WorkPlan-BUGFIXING.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Smalt and Beryl\Working Documents\Internship\Internship2018\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\D\NSKFDC BUG FIXING\NSKFDC\trunk\Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0FCAC848-347B-457D-95A1-2CBB789A4540}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9E2F04B7-A0BA-4288-8404-79D3BF83122E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8235" xr2:uid="{7B4AED39-2818-41CB-A4E7-8682F0B1C0D0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Populate the Training Partner name on the TP table | 2 hrs</t>
   </si>
@@ -154,12 +154,15 @@
   </si>
   <si>
     <t>Upload Functionality | Data Import | 2 hr</t>
+  </si>
+  <si>
+    <t>2+F1:O266</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -217,7 +220,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -266,8 +269,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -301,11 +310,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -325,7 +347,6 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -339,12 +360,46 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{1D369F45-D95A-4E32-9EC3-C707396AF034}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -653,20 +708,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D11B615-8310-4737-8444-29FCE8161971}">
-  <dimension ref="C1:H40"/>
+  <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="120.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="88.140625" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="4"/>
+      <c r="B1" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
@@ -676,118 +736,282 @@
       <c r="E1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="3">
+        <v>25</v>
+      </c>
+      <c r="G1" s="3">
+        <v>26</v>
+      </c>
+      <c r="H1" s="3">
+        <v>27</v>
+      </c>
+      <c r="I1" s="25">
+        <v>28</v>
+      </c>
+      <c r="J1" s="25">
+        <v>29</v>
+      </c>
+      <c r="K1" s="3">
+        <v>30</v>
+      </c>
+      <c r="L1" s="3">
+        <v>31</v>
+      </c>
+      <c r="M1" s="3">
+        <v>1</v>
+      </c>
+      <c r="N1" s="3">
+        <v>2</v>
+      </c>
+      <c r="O1" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="3">
         <v>2</v>
       </c>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="20"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="3">
         <v>1.5</v>
       </c>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="21">
+        <v>1.5</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="11" t="s">
+        <v>15</v>
+      </c>
       <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="3">
         <v>0.75</v>
       </c>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="20"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="3">
         <v>2.25</v>
       </c>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="20"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="3">
         <v>1.5</v>
       </c>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="20"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="3">
         <v>3</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="21">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="3">
         <v>1.5</v>
       </c>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E8" s="20"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="3">
         <v>1.5</v>
       </c>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E9" s="20"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="3">
         <v>0.75</v>
       </c>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E10" s="20"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="3">
         <v>0.75</v>
       </c>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E11" s="20"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="3">
         <v>7.5</v>
       </c>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E12" s="20"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="3">
         <v>3</v>
       </c>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E13" s="20"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C14" s="7" t="s">
         <v>20</v>
       </c>
@@ -795,254 +1019,533 @@
         <v>3</v>
       </c>
       <c r="E14" s="8"/>
-    </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C15" s="12"/>
       <c r="D15" s="12">
         <f>SUM(D2:D14)</f>
         <v>29</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15" s="22">
         <f>SUM(E2:E13)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C16" s="14" t="s">
+        <v>5.5</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C16" s="13" t="s">
         <v>16</v>
       </c>
       <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C17" s="15" t="s">
+      <c r="E16" s="23"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+    </row>
+    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C17" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D17" s="15">
         <v>2</v>
       </c>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C18" s="15" t="s">
+      <c r="E17" s="20"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+    </row>
+    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C18" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="16">
+      <c r="D18" s="15">
         <v>2.5</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="21">
         <v>2.75</v>
       </c>
-    </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C19" s="15" t="s">
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+    </row>
+    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C19" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="16">
+      <c r="D19" s="15">
         <v>0.75</v>
       </c>
-      <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C20" s="15" t="s">
+      <c r="E19" s="20"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+    </row>
+    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C20" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="16">
+      <c r="D20" s="15">
         <v>0.75</v>
       </c>
-      <c r="E20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C21" s="15" t="s">
+      <c r="E20" s="20"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+    </row>
+    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C21" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="16">
+      <c r="D21" s="15">
         <v>3</v>
       </c>
-      <c r="E21" s="4"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="15" t="s">
+      <c r="E21" s="20"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+    </row>
+    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C22" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="16">
+      <c r="D22" s="15">
         <v>1.5</v>
       </c>
-      <c r="E22" s="5"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C23" s="15" t="s">
+      <c r="E22" s="24">
+        <v>3</v>
+      </c>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+    </row>
+    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C23" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="16">
+      <c r="D23" s="15">
         <v>0.75</v>
       </c>
-      <c r="E23" s="4"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C24" s="15" t="s">
+      <c r="E23" s="20"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="25"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+    </row>
+    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C24" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="16">
+      <c r="D24" s="15">
         <v>1.5</v>
       </c>
-      <c r="E24" s="4"/>
-    </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C25" s="15" t="s">
+      <c r="E24" s="20"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+    </row>
+    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C25" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="16">
+      <c r="D25" s="15">
         <v>0.75</v>
       </c>
-      <c r="E25" s="4"/>
-    </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C26" s="17" t="s">
+      <c r="E25" s="20"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+    </row>
+    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C26" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="16">
+      <c r="D26" s="15">
         <v>4.5</v>
       </c>
-      <c r="E26" s="4"/>
-    </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C27" s="15" t="s">
+      <c r="E26" s="20"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+    </row>
+    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C27" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="16">
+      <c r="D27" s="15">
         <v>1.5</v>
       </c>
-      <c r="E27" s="4"/>
-    </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C28" s="15" t="s">
+      <c r="E27" s="20"/>
+      <c r="F27" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G27" s="3">
+        <v>26</v>
+      </c>
+      <c r="H27" s="3">
+        <v>27</v>
+      </c>
+      <c r="I27" s="25">
+        <v>28</v>
+      </c>
+      <c r="J27" s="25">
+        <v>29</v>
+      </c>
+      <c r="K27" s="3">
+        <v>30</v>
+      </c>
+      <c r="L27" s="3">
+        <v>31</v>
+      </c>
+      <c r="M27" s="3">
+        <v>1</v>
+      </c>
+      <c r="N27" s="3">
+        <v>2</v>
+      </c>
+      <c r="O27" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C28" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="16">
+      <c r="D28" s="15">
         <v>0.75</v>
       </c>
-      <c r="E28" s="4"/>
-    </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E28" s="20"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+    </row>
+    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C29" s="12"/>
       <c r="D29" s="12">
         <f>SUM(D17:D28)</f>
         <v>20.25</v>
       </c>
-      <c r="E29" s="12"/>
-    </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C30" s="18" t="s">
+      <c r="E29" s="22">
+        <f>SUM(E17:E28)</f>
+        <v>5.75</v>
+      </c>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="25"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+    </row>
+    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C30" s="17" t="s">
         <v>33</v>
       </c>
       <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-    </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E30" s="23"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="25"/>
+      <c r="J30" s="25"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+    </row>
+    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C31" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D31" s="3">
         <v>7.5</v>
       </c>
-      <c r="E31" s="4"/>
-    </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E31" s="20"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="25"/>
+      <c r="J31" s="25"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+    </row>
+    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C32" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D32" s="3">
         <v>6</v>
       </c>
-      <c r="E32" s="4"/>
-    </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E32" s="20"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="25"/>
+      <c r="J32" s="25"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+    </row>
+    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C33" s="3" t="s">
         <v>36</v>
       </c>
       <c r="D33" s="3">
         <v>2.5</v>
       </c>
-      <c r="E33" s="4"/>
-    </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="20"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="25"/>
+      <c r="J33" s="25"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+    </row>
+    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C34" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D34" s="3">
         <v>15</v>
       </c>
-      <c r="E34" s="4"/>
-    </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E34" s="20"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="25"/>
+      <c r="J34" s="25"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+    </row>
+    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C35" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D35" s="3">
         <v>3</v>
       </c>
-      <c r="E35" s="4"/>
-    </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C36" s="20" t="s">
+      <c r="E35" s="20"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="25"/>
+      <c r="J35" s="25"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
+    </row>
+    <row r="36" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C36" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="D36" s="19">
+      <c r="D36" s="18">
         <v>2</v>
       </c>
-      <c r="E36" s="4"/>
-    </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C37" s="20" t="s">
+      <c r="E36" s="20"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="25"/>
+      <c r="J36" s="25"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
+      <c r="O36" s="3"/>
+    </row>
+    <row r="37" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C37" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="D37" s="19">
+      <c r="D37" s="18">
         <v>1</v>
       </c>
-      <c r="E37" s="4"/>
-    </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E37" s="20"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="25"/>
+      <c r="J37" s="25"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
+      <c r="O37" s="3"/>
+    </row>
+    <row r="38" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C38" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D38" s="3">
         <v>1</v>
       </c>
-      <c r="E38" s="4"/>
-    </row>
-    <row r="39" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E38" s="20"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="25"/>
+      <c r="J38" s="25"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
+      <c r="O38" s="3"/>
+    </row>
+    <row r="39" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C39" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D39" s="3">
         <v>2</v>
       </c>
-      <c r="E39" s="4"/>
-    </row>
-    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E39" s="20"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="25"/>
+      <c r="J39" s="25"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+    </row>
+    <row r="40" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C40" s="12"/>
       <c r="D40" s="12">
         <f>SUM(D31:D39)</f>
         <v>40</v>
       </c>
-      <c r="E40" s="3"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="25"/>
+      <c r="J40" s="25"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="3"/>
+      <c r="O40" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Author        : Priyanka Chaudhary Description   : Updated Excel to prepare Gantt Chart File Updated  : WorkPlan-BUGFIXING.xlsx
</commit_message>
<xml_diff>
--- a/Requirements/WorkPlan-BUGFIXING.xlsx
+++ b/Requirements/WorkPlan-BUGFIXING.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\D\NSKFDC BUG FIXING\NSKFDC\trunk\Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9E2F04B7-A0BA-4288-8404-79D3BF83122E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1CD1200F-05D2-428E-8FEC-BB0867036C6B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8235" xr2:uid="{7B4AED39-2818-41CB-A4E7-8682F0B1C0D0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>Populate the Training Partner name on the TP table | 2 hrs</t>
   </si>
@@ -154,25 +154,14 @@
   </si>
   <si>
     <t>Upload Functionality | Data Import | 2 hr</t>
-  </si>
-  <si>
-    <t>2+F1:O266</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -215,12 +204,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -271,7 +261,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -327,45 +359,48 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -710,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D11B615-8310-4737-8444-29FCE8161971}">
   <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
+      <selection activeCell="Q28" sqref="Q28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,829 +758,861 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="4"/>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="3"/>
+      <c r="B1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="3">
+      <c r="F1" s="30">
         <v>25</v>
       </c>
-      <c r="G1" s="3">
+      <c r="G1" s="30">
         <v>26</v>
       </c>
-      <c r="H1" s="3">
+      <c r="H1" s="30">
         <v>27</v>
       </c>
-      <c r="I1" s="25">
+      <c r="I1" s="30">
         <v>28</v>
       </c>
-      <c r="J1" s="25">
+      <c r="J1" s="30">
         <v>29</v>
       </c>
-      <c r="K1" s="3">
+      <c r="K1" s="30">
         <v>30</v>
       </c>
-      <c r="L1" s="3">
+      <c r="L1" s="30">
         <v>31</v>
       </c>
-      <c r="M1" s="3">
+      <c r="M1" s="30">
         <v>1</v>
       </c>
-      <c r="N1" s="3">
+      <c r="N1" s="30">
         <v>2</v>
       </c>
-      <c r="O1" s="3">
+      <c r="O1" s="30">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>2</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="9"/>
+      <c r="B3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>1.5</v>
       </c>
-      <c r="E3" s="21">
+      <c r="E3" s="18">
         <v>1.5</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="11" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>0.75</v>
       </c>
-      <c r="E4" s="20"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>2.25</v>
       </c>
-      <c r="E5" s="20"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>1.5</v>
       </c>
-      <c r="E6" s="20"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>3</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="18">
         <v>4</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>1.5</v>
       </c>
-      <c r="E8" s="20"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>1.5</v>
       </c>
-      <c r="E9" s="20"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>0.75</v>
       </c>
-      <c r="E10" s="20"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>0.75</v>
       </c>
-      <c r="E11" s="20"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <v>7.5</v>
       </c>
-      <c r="E12" s="20"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <v>3</v>
       </c>
-      <c r="E13" s="20"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="8">
         <v>3</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C15" s="12"/>
-      <c r="D15" s="12">
+      <c r="C15" s="10"/>
+      <c r="D15" s="10">
         <f>SUM(D2:D14)</f>
         <v>29</v>
       </c>
-      <c r="E15" s="22">
+      <c r="E15" s="19">
         <f>SUM(E2:E13)</f>
         <v>5.5</v>
       </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
+      <c r="D16" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="30">
+        <v>25</v>
+      </c>
+      <c r="G16" s="30">
+        <v>26</v>
+      </c>
+      <c r="H16" s="30">
+        <v>27</v>
+      </c>
+      <c r="I16" s="30">
+        <v>28</v>
+      </c>
+      <c r="J16" s="30">
+        <v>29</v>
+      </c>
+      <c r="K16" s="30">
+        <v>30</v>
+      </c>
+      <c r="L16" s="30">
+        <v>31</v>
+      </c>
+      <c r="M16" s="30">
+        <v>1</v>
+      </c>
+      <c r="N16" s="30">
+        <v>2</v>
+      </c>
+      <c r="O16" s="30">
+        <v>3</v>
+      </c>
     </row>
     <row r="17" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="12">
         <v>2</v>
       </c>
-      <c r="E17" s="20"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
     </row>
     <row r="18" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="12">
         <v>2.5</v>
       </c>
-      <c r="E18" s="21">
+      <c r="E18" s="18">
         <v>2.75</v>
       </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
     </row>
     <row r="19" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D19" s="12">
         <v>0.75</v>
       </c>
-      <c r="E19" s="20"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
     </row>
     <row r="20" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="15">
+      <c r="D20" s="12">
         <v>0.75</v>
       </c>
-      <c r="E20" s="20"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
     </row>
     <row r="21" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="15">
+      <c r="D21" s="12">
         <v>3</v>
       </c>
-      <c r="E21" s="20"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
     </row>
     <row r="22" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="15">
+      <c r="D22" s="12">
         <v>1.5</v>
       </c>
-      <c r="E22" s="24">
+      <c r="E22" s="18">
         <v>3</v>
       </c>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="25"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
     </row>
     <row r="23" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="15">
+      <c r="D23" s="12">
         <v>0.75</v>
       </c>
-      <c r="E23" s="20"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
     </row>
     <row r="24" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="15">
+      <c r="D24" s="12">
         <v>1.5</v>
       </c>
-      <c r="E24" s="20"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="25"/>
-      <c r="J24" s="25"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="3"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
     </row>
     <row r="25" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="15">
+      <c r="D25" s="12">
         <v>0.75</v>
       </c>
-      <c r="E25" s="20"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="25"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
-      <c r="O25" s="3"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
     </row>
     <row r="26" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C26" s="16" t="s">
+      <c r="C26" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="15">
+      <c r="D26" s="12">
         <v>4.5</v>
       </c>
-      <c r="E26" s="20"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="25"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
-      <c r="O26" s="3"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
     </row>
     <row r="27" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="15">
+      <c r="D27" s="12">
         <v>1.5</v>
       </c>
-      <c r="E27" s="20"/>
-      <c r="F27" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G27" s="3">
-        <v>26</v>
-      </c>
-      <c r="H27" s="3">
-        <v>27</v>
-      </c>
-      <c r="I27" s="25">
-        <v>28</v>
-      </c>
-      <c r="J27" s="25">
-        <v>29</v>
-      </c>
-      <c r="K27" s="3">
-        <v>30</v>
-      </c>
-      <c r="L27" s="3">
-        <v>31</v>
-      </c>
-      <c r="M27" s="3">
-        <v>1</v>
-      </c>
-      <c r="N27" s="3">
-        <v>2</v>
-      </c>
-      <c r="O27" s="3">
-        <v>3</v>
-      </c>
+      <c r="E27" s="17"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
     </row>
     <row r="28" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="15">
+      <c r="D28" s="12">
         <v>0.75</v>
       </c>
-      <c r="E28" s="20"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
-      <c r="O28" s="3"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
     </row>
     <row r="29" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C29" s="12"/>
-      <c r="D29" s="12">
+      <c r="C29" s="10"/>
+      <c r="D29" s="10">
         <f>SUM(D17:D28)</f>
         <v>20.25</v>
       </c>
-      <c r="E29" s="22">
+      <c r="E29" s="19">
         <f>SUM(E17:E28)</f>
         <v>5.75</v>
       </c>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
-      <c r="O29" s="3"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
     </row>
     <row r="30" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C30" s="17" t="s">
+      <c r="C30" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="D30" s="3"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="25"/>
-      <c r="J30" s="25"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
-      <c r="O30" s="3"/>
+      <c r="D30" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" s="30">
+        <v>25</v>
+      </c>
+      <c r="G30" s="30">
+        <v>26</v>
+      </c>
+      <c r="H30" s="30">
+        <v>27</v>
+      </c>
+      <c r="I30" s="30">
+        <v>28</v>
+      </c>
+      <c r="J30" s="30">
+        <v>29</v>
+      </c>
+      <c r="K30" s="30">
+        <v>30</v>
+      </c>
+      <c r="L30" s="30">
+        <v>31</v>
+      </c>
+      <c r="M30" s="30">
+        <v>1</v>
+      </c>
+      <c r="N30" s="30">
+        <v>2</v>
+      </c>
+      <c r="O30" s="30">
+        <v>3</v>
+      </c>
     </row>
     <row r="31" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31" s="2">
         <v>7.5</v>
       </c>
-      <c r="E31" s="20"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="25"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
-      <c r="O31" s="3"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
     </row>
     <row r="32" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D32" s="2">
         <v>6</v>
       </c>
-      <c r="E32" s="20"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="25"/>
-      <c r="J32" s="25"/>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
-      <c r="M32" s="3"/>
-      <c r="N32" s="3"/>
-      <c r="O32" s="3"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="21"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
     </row>
     <row r="33" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D33" s="2">
         <v>2.5</v>
       </c>
-      <c r="E33" s="20"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="25"/>
-      <c r="J33" s="25"/>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
-      <c r="M33" s="3"/>
-      <c r="N33" s="3"/>
-      <c r="O33" s="3"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="21"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
     </row>
     <row r="34" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34" s="2">
         <v>15</v>
       </c>
-      <c r="E34" s="20"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="25"/>
-      <c r="J34" s="25"/>
-      <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
-      <c r="M34" s="3"/>
-      <c r="N34" s="3"/>
-      <c r="O34" s="3"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
     </row>
     <row r="35" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D35" s="2">
         <v>3</v>
       </c>
-      <c r="E35" s="20"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="25"/>
-      <c r="J35" s="25"/>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
-      <c r="M35" s="3"/>
-      <c r="N35" s="3"/>
-      <c r="O35" s="3"/>
+      <c r="E35" s="18">
+        <v>1</v>
+      </c>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="21"/>
+      <c r="J35" s="21"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
     </row>
     <row r="36" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C36" s="19" t="s">
+      <c r="C36" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="D36" s="18">
+      <c r="D36" s="14">
         <v>2</v>
       </c>
-      <c r="E36" s="20"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="25"/>
-      <c r="J36" s="25"/>
-      <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
-      <c r="M36" s="3"/>
-      <c r="N36" s="3"/>
-      <c r="O36" s="3"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="21"/>
+      <c r="J36" s="21"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
     </row>
     <row r="37" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C37" s="19" t="s">
+      <c r="C37" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="D37" s="18">
+      <c r="D37" s="14">
         <v>1</v>
       </c>
-      <c r="E37" s="20"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="25"/>
-      <c r="J37" s="25"/>
-      <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
-      <c r="M37" s="3"/>
-      <c r="N37" s="3"/>
-      <c r="O37" s="3"/>
+      <c r="E37" s="18">
+        <v>3</v>
+      </c>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="21"/>
+      <c r="J37" s="21"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
     </row>
     <row r="38" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D38" s="3">
+      <c r="D38" s="2">
         <v>1</v>
       </c>
-      <c r="E38" s="20"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="25"/>
-      <c r="J38" s="25"/>
-      <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
-      <c r="M38" s="3"/>
-      <c r="N38" s="3"/>
-      <c r="O38" s="3"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="21"/>
+      <c r="J38" s="21"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
     </row>
     <row r="39" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D39" s="2">
         <v>2</v>
       </c>
-      <c r="E39" s="20"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="25"/>
-      <c r="J39" s="25"/>
-      <c r="K39" s="3"/>
-      <c r="L39" s="3"/>
-      <c r="M39" s="3"/>
-      <c r="N39" s="3"/>
-      <c r="O39" s="3"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="21"/>
+      <c r="J39" s="21"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
     </row>
     <row r="40" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C40" s="12"/>
-      <c r="D40" s="12">
+      <c r="C40" s="10"/>
+      <c r="D40" s="10">
         <f>SUM(D31:D39)</f>
         <v>40</v>
       </c>
-      <c r="E40" s="23"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="25"/>
-      <c r="J40" s="25"/>
-      <c r="K40" s="3"/>
-      <c r="L40" s="3"/>
-      <c r="M40" s="3"/>
-      <c r="N40" s="3"/>
-      <c r="O40" s="3"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="21"/>
+      <c r="J40" s="21"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Author:           Pooja Sharma Files Modified:   WorkPlan-BUGFIXING.xlsx Description:      Gantt chart updated
</commit_message>
<xml_diff>
--- a/Requirements/WorkPlan-BUGFIXING.xlsx
+++ b/Requirements/WorkPlan-BUGFIXING.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\NSKFDC-App.git\trunk\Requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NSKFDC-App.git\trunk\Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{04F4F8C8-22D1-4B98-997F-97C4F83DF247}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="8232" xr2:uid="{7B4AED39-2818-41CB-A4E7-8682F0B1C0D0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="8232"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>Populate the Training Partner name on the TP table | 2 hrs</t>
   </si>
@@ -154,19 +156,13 @@
   </si>
   <si>
     <t>Upload Functionality | Data Import | 2 hr</t>
-  </si>
-  <si>
-    <t>SCGJ Proposal | Pravek</t>
-  </si>
-  <si>
-    <t>NSKFDC App Deplyment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -215,15 +211,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="22">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -320,35 +309,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -398,11 +358,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -428,6 +387,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -443,14 +403,8 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -478,7 +432,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{1D369F45-D95A-4E32-9EC3-C707396AF034}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -790,11 +744,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D11B615-8310-4737-8444-29FCE8161971}">
-  <dimension ref="A1:O42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B18" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="M40" sqref="M40"/>
+    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -802,7 +756,7 @@
     <col min="2" max="2" width="19.5546875" customWidth="1"/>
     <col min="3" max="3" width="88.109375" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="28.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -810,43 +764,43 @@
       <c r="B1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="28">
+      <c r="F1" s="29">
         <v>25</v>
       </c>
-      <c r="G1" s="28">
+      <c r="G1" s="29">
         <v>26</v>
       </c>
-      <c r="H1" s="28">
+      <c r="H1" s="29">
         <v>27</v>
       </c>
-      <c r="I1" s="28">
+      <c r="I1" s="29">
         <v>28</v>
       </c>
-      <c r="J1" s="28">
+      <c r="J1" s="29">
         <v>29</v>
       </c>
-      <c r="K1" s="28">
+      <c r="K1" s="29">
         <v>30</v>
       </c>
-      <c r="L1" s="28">
+      <c r="L1" s="29">
         <v>31</v>
       </c>
-      <c r="M1" s="28">
+      <c r="M1" s="29">
         <v>1</v>
       </c>
-      <c r="N1" s="28">
+      <c r="N1" s="29">
         <v>2</v>
       </c>
-      <c r="O1" s="28">
+      <c r="O1" s="29">
         <v>3</v>
       </c>
     </row>
@@ -864,10 +818,10 @@
       <c r="E2" s="16"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="20"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="21"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -887,11 +841,11 @@
       <c r="E3" s="17">
         <v>1.5</v>
       </c>
-      <c r="F3" s="21"/>
+      <c r="F3" s="22"/>
       <c r="G3" s="2"/>
       <c r="H3" s="12"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -911,10 +865,10 @@
       </c>
       <c r="E4" s="16"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="23"/>
+      <c r="G4" s="24"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -932,10 +886,10 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
       <c r="K5" s="12"/>
-      <c r="L5" s="24"/>
+      <c r="L5" s="25"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -951,9 +905,9 @@
       <c r="F6" s="12"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="21"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -969,11 +923,11 @@
       <c r="E7" s="17">
         <v>4</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="22"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -989,12 +943,12 @@
       </c>
       <c r="E8" s="16"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="22"/>
+      <c r="G8" s="23"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
       <c r="K8" s="12"/>
-      <c r="L8" s="24"/>
+      <c r="L8" s="25"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
@@ -1008,10 +962,10 @@
       </c>
       <c r="E9" s="16"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="23"/>
+      <c r="G9" s="24"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -1027,10 +981,10 @@
       </c>
       <c r="E10" s="16"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="23"/>
+      <c r="G10" s="24"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
@@ -1047,9 +1001,9 @@
       <c r="E11" s="16"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
@@ -1065,10 +1019,10 @@
       </c>
       <c r="E12" s="16"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
@@ -1086,9 +1040,9 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="21"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -1105,8 +1059,8 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
@@ -1123,55 +1077,55 @@
         <f>SUM(E2:E13)</f>
         <v>5.5</v>
       </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="D16" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="26" t="s">
+      <c r="E16" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="28">
+      <c r="F16" s="29">
         <v>25</v>
       </c>
-      <c r="G16" s="28">
+      <c r="G16" s="29">
         <v>26</v>
       </c>
-      <c r="H16" s="28">
+      <c r="H16" s="29">
         <v>27</v>
       </c>
-      <c r="I16" s="28">
+      <c r="I16" s="29">
         <v>28</v>
       </c>
-      <c r="J16" s="28">
+      <c r="J16" s="29">
         <v>29</v>
       </c>
-      <c r="K16" s="28">
+      <c r="K16" s="29">
         <v>30</v>
       </c>
-      <c r="L16" s="28">
+      <c r="L16" s="29">
         <v>31</v>
       </c>
-      <c r="M16" s="28">
+      <c r="M16" s="29">
         <v>1</v>
       </c>
-      <c r="N16" s="28">
+      <c r="N16" s="29">
         <v>2</v>
       </c>
-      <c r="O16" s="28">
+      <c r="O16" s="29">
         <v>3</v>
       </c>
     </row>
@@ -1186,9 +1140,9 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="2"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="21"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -1204,11 +1158,11 @@
       <c r="E18" s="17">
         <v>2.75</v>
       </c>
-      <c r="F18" s="2"/>
+      <c r="F18" s="22"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
@@ -1223,11 +1177,11 @@
         <v>0.75</v>
       </c>
       <c r="E19" s="16"/>
-      <c r="F19" s="2"/>
+      <c r="F19" s="22"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
@@ -1242,11 +1196,11 @@
         <v>0.75</v>
       </c>
       <c r="E20" s="16"/>
-      <c r="F20" s="2"/>
+      <c r="F20" s="22"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
@@ -1262,10 +1216,10 @@
       </c>
       <c r="E21" s="16"/>
       <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+      <c r="G21" s="24"/>
       <c r="H21" s="2"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
@@ -1282,11 +1236,11 @@
       <c r="E22" s="17">
         <v>3</v>
       </c>
-      <c r="F22" s="2"/>
+      <c r="F22" s="22"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
@@ -1302,10 +1256,10 @@
       </c>
       <c r="E23" s="16"/>
       <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="G23" s="24"/>
       <c r="H23" s="2"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
@@ -1321,10 +1275,10 @@
       </c>
       <c r="E24" s="16"/>
       <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
+      <c r="G24" s="24"/>
       <c r="H24" s="2"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="19"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
@@ -1340,10 +1294,10 @@
       </c>
       <c r="E25" s="16"/>
       <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
+      <c r="G25" s="24"/>
       <c r="H25" s="2"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
@@ -1360,9 +1314,9 @@
       <c r="E26" s="16"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="19"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
@@ -1379,9 +1333,9 @@
       <c r="E27" s="16"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="19"/>
-      <c r="J27" s="19"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
@@ -1395,14 +1349,12 @@
       <c r="D28" s="12">
         <v>0.75</v>
       </c>
-      <c r="E28" s="17">
-        <v>0.5</v>
-      </c>
-      <c r="F28" s="2"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="22"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
@@ -1417,57 +1369,57 @@
       </c>
       <c r="E29" s="18">
         <f>SUM(E17:E28)</f>
-        <v>6.25</v>
-      </c>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="10"/>
-      <c r="M29" s="10"/>
-      <c r="N29" s="10"/>
-      <c r="O29" s="10"/>
+        <v>5.75</v>
+      </c>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
     </row>
     <row r="30" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C30" s="27" t="s">
+      <c r="C30" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="D30" s="26" t="s">
+      <c r="D30" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E30" s="26" t="s">
+      <c r="E30" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F30" s="28">
+      <c r="F30" s="29">
         <v>25</v>
       </c>
-      <c r="G30" s="28">
+      <c r="G30" s="29">
         <v>26</v>
       </c>
-      <c r="H30" s="28">
+      <c r="H30" s="29">
         <v>27</v>
       </c>
-      <c r="I30" s="28">
+      <c r="I30" s="29">
         <v>28</v>
       </c>
-      <c r="J30" s="28">
+      <c r="J30" s="29">
         <v>29</v>
       </c>
-      <c r="K30" s="28">
+      <c r="K30" s="29">
         <v>30</v>
       </c>
-      <c r="L30" s="28">
+      <c r="L30" s="29">
         <v>31</v>
       </c>
-      <c r="M30" s="28">
+      <c r="M30" s="29">
         <v>1</v>
       </c>
-      <c r="N30" s="28">
+      <c r="N30" s="29">
         <v>2</v>
       </c>
-      <c r="O30" s="28">
+      <c r="O30" s="29">
         <v>3</v>
       </c>
     </row>
@@ -1481,9 +1433,10 @@
       <c r="E31" s="16"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
-      <c r="H31" s="30"/>
-      <c r="I31" s="30"/>
-      <c r="J31" s="19"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="2"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -1500,12 +1453,12 @@
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
-      <c r="M32" s="21"/>
-      <c r="N32" s="21"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
       <c r="O32" s="2"/>
     </row>
     <row r="33" spans="3:15" x14ac:dyDescent="0.3">
@@ -1517,10 +1470,10 @@
       </c>
       <c r="E33" s="16"/>
       <c r="F33" s="2"/>
-      <c r="G33" s="5"/>
+      <c r="G33" s="2"/>
       <c r="H33" s="2"/>
-      <c r="I33" s="19"/>
-      <c r="J33" s="19"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="20"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
@@ -1538,11 +1491,11 @@
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
-      <c r="I34" s="19"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="31"/>
-      <c r="L34" s="31"/>
-      <c r="M34" s="31"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="20"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
     </row>
@@ -1556,11 +1509,11 @@
       <c r="E35" s="17">
         <v>1</v>
       </c>
-      <c r="F35" s="31"/>
+      <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
-      <c r="I35" s="19"/>
-      <c r="J35" s="19"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="20"/>
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
@@ -1574,14 +1527,12 @@
       <c r="D36" s="14">
         <v>2</v>
       </c>
-      <c r="E36" s="17">
-        <v>1</v>
-      </c>
-      <c r="F36" s="31"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
-      <c r="I36" s="19"/>
-      <c r="J36" s="19"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="20"/>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
@@ -1598,11 +1549,11 @@
       <c r="E37" s="17">
         <v>3</v>
       </c>
-      <c r="F37" s="31"/>
+      <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
-      <c r="I37" s="19"/>
-      <c r="J37" s="19"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="20"/>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
@@ -1617,10 +1568,11 @@
         <v>1</v>
       </c>
       <c r="E38" s="16"/>
-      <c r="G38" s="5"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
       <c r="H38" s="2"/>
-      <c r="I38" s="19"/>
-      <c r="J38" s="19"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="20"/>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
@@ -1634,13 +1586,12 @@
       <c r="D39" s="2">
         <v>2</v>
       </c>
-      <c r="E39" s="32">
-        <v>0.5</v>
-      </c>
-      <c r="G39" s="31"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
       <c r="H39" s="2"/>
-      <c r="I39" s="19"/>
-      <c r="J39" s="19"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="20"/>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
@@ -1648,61 +1599,22 @@
       <c r="O39" s="2"/>
     </row>
     <row r="40" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C40" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D40" s="2">
-        <v>6</v>
-      </c>
-      <c r="E40" s="16"/>
-      <c r="G40" s="12"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10">
+        <f>SUM(D31:D39)</f>
+        <v>40</v>
+      </c>
+      <c r="E40" s="19"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
       <c r="H40" s="2"/>
-      <c r="I40" s="19"/>
-      <c r="J40" s="19"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="20"/>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
-      <c r="O40" s="34"/>
-    </row>
-    <row r="41" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C41" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D41" s="2">
-        <v>1</v>
-      </c>
-      <c r="E41" s="16"/>
-      <c r="G41" s="33"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="19"/>
-      <c r="J41" s="19"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
-      <c r="M41" s="2"/>
-      <c r="N41" s="2"/>
-      <c r="O41" s="2"/>
-    </row>
-    <row r="42" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C42" s="10"/>
-      <c r="D42" s="10">
-        <f>SUM(D31:D41)</f>
-        <v>47</v>
-      </c>
-      <c r="E42" s="18">
-        <f>SUM(E31:E39)</f>
-        <v>5.5</v>
-      </c>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10"/>
-      <c r="I42" s="10"/>
-      <c r="J42" s="10"/>
-      <c r="K42" s="10"/>
-      <c r="L42" s="10"/>
-      <c r="M42" s="10"/>
-      <c r="N42" s="10"/>
-      <c r="O42" s="10"/>
+      <c r="O40" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Author        : Priyanka Chaudhary Description   : Updated Logs File Updated  : WorkPlan-BUGFIXING.xlsx
</commit_message>
<xml_diff>
--- a/Requirements/WorkPlan-BUGFIXING.xlsx
+++ b/Requirements/WorkPlan-BUGFIXING.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\D\NSKFDC BUG FIXING\NSKFDC\trunk\Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B27E477D-DC87-4273-AD95-7AC679A2615B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5BFCE2EE-CB2E-4067-8E5E-F4D1F7C52FE7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="84">
   <si>
     <t>Populate the Training Partner name on the TP table | 2 hrs</t>
   </si>
@@ -271,13 +271,22 @@
   </si>
   <si>
     <t>NA-18</t>
+  </si>
+  <si>
+    <t>Delay</t>
+  </si>
+  <si>
+    <t>NA-96</t>
+  </si>
+  <si>
+    <t>JIRA Monitoring</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -333,8 +342,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="22">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -456,12 +473,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -510,29 +533,17 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -540,25 +551,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -575,16 +580,31 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -929,10 +949,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P42"/>
+  <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
-      <selection activeCell="R25" sqref="R25"/>
+    <sheetView tabSelected="1" topLeftCell="C8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,1020 +961,1222 @@
     <col min="4" max="4" width="88.140625" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="28.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" style="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="16">
+      <c r="G1" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="H1" s="43">
         <v>25</v>
       </c>
-      <c r="H1" s="16">
+      <c r="I1" s="13">
         <v>26</v>
       </c>
-      <c r="I1" s="16">
+      <c r="J1" s="13">
         <v>27</v>
       </c>
-      <c r="J1" s="16">
+      <c r="K1" s="13">
         <v>28</v>
       </c>
-      <c r="K1" s="16">
+      <c r="L1" s="13">
         <v>29</v>
       </c>
-      <c r="L1" s="16">
+      <c r="M1" s="13">
         <v>30</v>
       </c>
-      <c r="M1" s="16">
+      <c r="N1" s="13">
         <v>31</v>
       </c>
-      <c r="N1" s="16">
+      <c r="O1" s="13">
         <v>1</v>
       </c>
-      <c r="O1" s="16">
+      <c r="P1" s="13">
         <v>2</v>
       </c>
-      <c r="P1" s="16">
+      <c r="Q1" s="13">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="32">
+      <c r="E2" s="25">
         <v>2</v>
       </c>
-      <c r="F2" s="42"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="1"/>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="45">
+        <f>(E2-F2)</f>
+        <v>2</v>
+      </c>
+      <c r="H2" s="17"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="9"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="38" t="s">
+      <c r="Q2" s="1"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="32">
+      <c r="E3" s="25">
         <v>1.5</v>
       </c>
-      <c r="F3" s="43">
+      <c r="F3" s="41">
         <v>1.5</v>
       </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="1"/>
+      <c r="G3" s="45">
+        <f t="shared" ref="G3:G43" si="0">(E3-F3)</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="38"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q3" s="1"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="32">
+      <c r="E4" s="25">
         <v>0.75</v>
       </c>
-      <c r="F4" s="44"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="1"/>
+      <c r="F4" s="40">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="45">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="H4" s="17"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C5" s="35" t="s">
+      <c r="Q4" s="1"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C5" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="32">
+      <c r="E5" s="25">
         <v>2.25</v>
       </c>
-      <c r="F5" s="42"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="45">
+        <f t="shared" si="0"/>
+        <v>2.25</v>
+      </c>
+      <c r="H5" s="17"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="12"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C6" s="35" t="s">
+      <c r="Q5" s="1"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C6" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="25">
         <v>1.5</v>
       </c>
-      <c r="F6" s="42"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="1"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="45">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="H6" s="37"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="9"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C7" s="32" t="s">
+      <c r="Q6" s="1"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C7" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="D7" s="31" t="s">
+      <c r="D7" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="32">
+      <c r="E7" s="25">
         <v>3</v>
       </c>
-      <c r="F7" s="43">
+      <c r="F7" s="41">
         <v>4</v>
       </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="1"/>
+      <c r="G7" s="45">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="H7" s="38"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C8" s="32" t="s">
+      <c r="Q7" s="1"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C8" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="25">
         <v>1.5</v>
       </c>
-      <c r="F8" s="42"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="1"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="45">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="H8" s="17"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="12"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C9" s="32" t="s">
+      <c r="Q8" s="1"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C9" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="32">
+      <c r="E9" s="25">
         <v>1.5</v>
       </c>
-      <c r="F9" s="42"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="1"/>
+      <c r="F9" s="40">
+        <v>0.5</v>
+      </c>
+      <c r="G9" s="45">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H9" s="17"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C10" s="32" t="s">
+      <c r="Q9" s="1"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C10" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="31" t="s">
+      <c r="D10" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="32">
+      <c r="E10" s="25">
         <v>0.75</v>
       </c>
-      <c r="F10" s="42"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="1"/>
+      <c r="F10" s="40">
+        <v>0.5</v>
+      </c>
+      <c r="G10" s="45">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="H10" s="17"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C11" s="32" t="s">
+      <c r="Q10" s="1"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C11" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="32">
+      <c r="E11" s="25">
         <v>0.75</v>
       </c>
-      <c r="F11" s="42"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="1"/>
+      <c r="F11" s="40">
+        <v>1</v>
+      </c>
+      <c r="G11" s="45">
+        <f t="shared" si="0"/>
+        <v>-0.25</v>
+      </c>
+      <c r="H11" s="17"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C12" s="32" t="s">
+      <c r="Q11" s="1"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C12" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="31" t="s">
+      <c r="D12" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="32">
+      <c r="E12" s="25">
         <v>7.5</v>
       </c>
-      <c r="F12" s="42"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="1"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="45">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+      <c r="H12" s="17"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C13" s="32" t="s">
+      <c r="Q12" s="1"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C13" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="32">
+      <c r="E13" s="25">
         <v>3</v>
       </c>
-      <c r="F13" s="42"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="45">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H13" s="17"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="9"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C14" s="32" t="s">
+      <c r="Q13" s="1"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C14" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="31" t="s">
+      <c r="D14" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="35">
+      <c r="E14" s="28">
         <v>3</v>
       </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="45">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H14" s="17"/>
       <c r="I14" s="1"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
       <c r="M14" s="1"/>
-      <c r="N14" s="19"/>
-      <c r="O14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="16"/>
       <c r="P14" s="1"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C15" s="32"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33">
-        <f>SUM(E2:E14)</f>
+      <c r="Q14" s="1"/>
+    </row>
+    <row r="15" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" s="28"/>
+      <c r="F15" s="3">
+        <v>2</v>
+      </c>
+      <c r="G15" s="45"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="25"/>
+      <c r="N15" s="25"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="25"/>
+      <c r="Q15" s="25"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C16" s="25"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26">
+        <f>SUM(E2:E15)</f>
         <v>29</v>
       </c>
-      <c r="F15" s="45">
-        <f>SUM(F2:F13)</f>
-        <v>5.5</v>
-      </c>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C16" s="50" t="s">
+      <c r="F16" s="26">
+        <f>SUM(F2:F15)</f>
+        <v>10</v>
+      </c>
+      <c r="G16" s="46">
+        <f>(E16-F16)</f>
+        <v>19</v>
+      </c>
+      <c r="H16" s="17"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+    </row>
+    <row r="17" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C17" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="40" t="s">
+      <c r="D17" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="41" t="s">
+      <c r="E17" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="F17" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="16">
+      <c r="G17" s="45"/>
+      <c r="H17" s="43">
         <v>25</v>
       </c>
-      <c r="H16" s="16">
+      <c r="I17" s="13">
         <v>26</v>
       </c>
-      <c r="I16" s="16">
+      <c r="J17" s="13">
         <v>27</v>
       </c>
-      <c r="J16" s="16">
+      <c r="K17" s="13">
         <v>28</v>
       </c>
-      <c r="K16" s="16">
+      <c r="L17" s="13">
         <v>29</v>
       </c>
-      <c r="L16" s="16">
+      <c r="M17" s="13">
         <v>30</v>
       </c>
-      <c r="M16" s="16">
+      <c r="N17" s="13">
         <v>31</v>
       </c>
-      <c r="N16" s="16">
+      <c r="O17" s="13">
         <v>1</v>
       </c>
-      <c r="O16" s="16">
+      <c r="P17" s="13">
         <v>2</v>
       </c>
-      <c r="P16" s="16">
+      <c r="Q17" s="13">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C17" s="32" t="s">
+    <row r="18" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C18" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="D17" s="34" t="s">
+      <c r="D18" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="35">
+      <c r="E18" s="28">
         <v>2</v>
       </c>
-      <c r="F17" s="42"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-    </row>
-    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C18" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="D18" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="E18" s="35">
-        <v>2.5</v>
-      </c>
-      <c r="F18" s="43">
-        <v>2.75</v>
-      </c>
-      <c r="G18" s="11"/>
-      <c r="H18" s="1"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="45">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H18" s="17"/>
       <c r="I18" s="1"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="9"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
-    </row>
-    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C19" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="D19" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19" s="35">
-        <v>0.75</v>
-      </c>
-      <c r="F19" s="42">
-        <v>0.75</v>
-      </c>
-      <c r="G19" s="11"/>
-      <c r="H19" s="1"/>
+      <c r="Q18" s="1"/>
+    </row>
+    <row r="19" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C19" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="28">
+        <v>2.5</v>
+      </c>
+      <c r="F19" s="41">
+        <v>2.75</v>
+      </c>
+      <c r="G19" s="47">
+        <f t="shared" si="0"/>
+        <v>-0.25</v>
+      </c>
+      <c r="H19" s="38"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="39"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
-    </row>
-    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C20" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="D20" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="E20" s="35">
+      <c r="Q19" s="1"/>
+    </row>
+    <row r="20" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C20" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="28">
         <v>0.75</v>
       </c>
-      <c r="F20" s="43">
+      <c r="F20" s="2">
         <v>0.75</v>
       </c>
-      <c r="G20" s="11"/>
-      <c r="H20" s="1"/>
+      <c r="G20" s="47">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H20" s="38"/>
       <c r="I20" s="1"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="32"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
-    </row>
-    <row r="21" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C21" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="D21" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="E21" s="35">
-        <v>3</v>
-      </c>
-      <c r="F21" s="42"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="13"/>
+      <c r="Q20" s="1"/>
+    </row>
+    <row r="21" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C21" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="28">
+        <v>0.75</v>
+      </c>
+      <c r="F21" s="41">
+        <v>0.75</v>
+      </c>
+      <c r="G21" s="47">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H21" s="38"/>
       <c r="I21" s="1"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
-    </row>
-    <row r="22" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C22" s="32" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22" s="35">
-        <v>1.5</v>
-      </c>
-      <c r="F22" s="43">
+      <c r="Q21" s="1"/>
+    </row>
+    <row r="22" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C22" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="28">
         <v>3</v>
       </c>
-      <c r="G22" s="11"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="1"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="45">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H22" s="17"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
-    </row>
-    <row r="23" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C23" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="D23" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="E23" s="35">
-        <v>0.75</v>
-      </c>
-      <c r="F23" s="44"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="13"/>
+      <c r="Q22" s="1"/>
+    </row>
+    <row r="23" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C23" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="28">
+        <v>1.5</v>
+      </c>
+      <c r="F23" s="41">
+        <v>3</v>
+      </c>
+      <c r="G23" s="47">
+        <f t="shared" si="0"/>
+        <v>-1.5</v>
+      </c>
+      <c r="H23" s="38"/>
       <c r="I23" s="1"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
-    </row>
-    <row r="24" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C24" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="D24" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="E24" s="35">
-        <v>1.5</v>
-      </c>
-      <c r="F24" s="42"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="1"/>
+      <c r="Q23" s="1"/>
+    </row>
+    <row r="24" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C24" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" s="28">
+        <v>0.75</v>
+      </c>
+      <c r="F24" s="41">
+        <v>0.75</v>
+      </c>
+      <c r="G24" s="45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H24" s="17"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
-    </row>
-    <row r="25" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C25" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="D25" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="E25" s="35">
-        <v>0.75</v>
-      </c>
-      <c r="F25" s="42"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="1"/>
+      <c r="Q24" s="1"/>
+    </row>
+    <row r="25" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C25" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="28">
+        <v>1.5</v>
+      </c>
+      <c r="F25" s="2"/>
+      <c r="G25" s="45">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="H25" s="17"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
-    </row>
-    <row r="26" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C26" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E26" s="35">
-        <v>4.5</v>
-      </c>
-      <c r="F26" s="42"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
-      <c r="L26" s="1"/>
+      <c r="Q25" s="1"/>
+    </row>
+    <row r="26" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C26" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" s="28">
+        <v>0.75</v>
+      </c>
+      <c r="F26" s="41">
+        <v>0.75</v>
+      </c>
+      <c r="G26" s="45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H26" s="17"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
-    </row>
-    <row r="27" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C27" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="D27" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="E27" s="35">
-        <v>1.5</v>
-      </c>
-      <c r="F27" s="42"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="1"/>
+      <c r="Q26" s="1"/>
+    </row>
+    <row r="27" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C27" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" s="28">
+        <v>4.5</v>
+      </c>
+      <c r="F27" s="3"/>
+      <c r="G27" s="45">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+      <c r="H27" s="17"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
-    </row>
-    <row r="28" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C28" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="D28" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="E28" s="35">
-        <v>0.75</v>
-      </c>
-      <c r="F28" s="43">
-        <v>0.5</v>
-      </c>
-      <c r="G28" s="11"/>
-      <c r="H28" s="1"/>
+      <c r="Q27" s="1"/>
+    </row>
+    <row r="28" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C28" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" s="28">
+        <v>1.5</v>
+      </c>
+      <c r="F28" s="2"/>
+      <c r="G28" s="45">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="H28" s="17"/>
       <c r="I28" s="1"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="1"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
-    </row>
-    <row r="29" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C29" s="32"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33">
-        <f>SUM(E17:E28)</f>
-        <v>20.25</v>
-      </c>
-      <c r="F29" s="45">
-        <f>SUM(F17:F28)</f>
-        <v>7.75</v>
-      </c>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
+      <c r="Q28" s="1"/>
+    </row>
+    <row r="29" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C29" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E29" s="28">
+        <v>0.75</v>
+      </c>
+      <c r="F29" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="G29" s="47">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="H29" s="38"/>
       <c r="I29" s="1"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
-    </row>
-    <row r="30" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C30" s="50" t="s">
+      <c r="Q29" s="1"/>
+    </row>
+    <row r="30" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C30" s="25"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26">
+        <f>SUM(E18:E29)</f>
+        <v>20.25</v>
+      </c>
+      <c r="F30" s="26">
+        <f>SUM(F18:F29)</f>
+        <v>9.25</v>
+      </c>
+      <c r="G30" s="46">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="H30" s="17"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+    </row>
+    <row r="31" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C31" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="40" t="s">
+      <c r="D31" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="E30" s="41" t="s">
+      <c r="E31" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F30" s="15" t="s">
+      <c r="F31" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G30" s="16">
+      <c r="G31" s="45"/>
+      <c r="H31" s="43">
         <v>25</v>
       </c>
-      <c r="H30" s="16">
+      <c r="I31" s="13">
         <v>26</v>
       </c>
-      <c r="I30" s="16">
+      <c r="J31" s="13">
         <v>27</v>
       </c>
-      <c r="J30" s="16">
+      <c r="K31" s="13">
         <v>28</v>
       </c>
-      <c r="K30" s="16">
+      <c r="L31" s="13">
         <v>29</v>
       </c>
-      <c r="L30" s="16">
+      <c r="M31" s="13">
         <v>30</v>
       </c>
-      <c r="M30" s="16">
+      <c r="N31" s="13">
         <v>31</v>
       </c>
-      <c r="N30" s="16">
+      <c r="O31" s="13">
         <v>1</v>
       </c>
-      <c r="O30" s="16">
+      <c r="P31" s="13">
         <v>2</v>
       </c>
-      <c r="P30" s="16">
+      <c r="Q31" s="13">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C31" s="32" t="s">
+    <row r="32" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C32" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="D31" s="32" t="s">
+      <c r="D32" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E31" s="32">
+      <c r="E32" s="25">
         <v>7.5</v>
       </c>
-      <c r="F31" s="46"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="27"/>
-      <c r="K31" s="25"/>
-      <c r="L31" s="22"/>
-      <c r="M31" s="23"/>
-      <c r="N31" s="23"/>
-      <c r="O31" s="23"/>
-      <c r="P31" s="23"/>
-    </row>
-    <row r="32" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C32" s="32" t="s">
+      <c r="F32" s="2"/>
+      <c r="G32" s="45">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+      <c r="H32" s="17"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="22"/>
+      <c r="L32" s="21"/>
+      <c r="M32" s="18"/>
+      <c r="N32" s="19"/>
+      <c r="O32" s="19"/>
+      <c r="P32" s="19"/>
+      <c r="Q32" s="19"/>
+    </row>
+    <row r="33" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C33" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="D32" s="32" t="s">
+      <c r="D33" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="E32" s="32">
+      <c r="E33" s="25">
         <v>6</v>
       </c>
-      <c r="F32" s="46"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="23"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="25"/>
-      <c r="K32" s="25"/>
-      <c r="L32" s="23"/>
-      <c r="M32" s="23"/>
-      <c r="N32" s="26"/>
-      <c r="O32" s="26"/>
-      <c r="P32" s="23"/>
-    </row>
-    <row r="33" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C33" s="32" t="s">
+      <c r="F33" s="2"/>
+      <c r="G33" s="45">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="H33" s="17"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="21"/>
+      <c r="L33" s="21"/>
+      <c r="M33" s="19"/>
+      <c r="N33" s="19"/>
+      <c r="O33" s="29"/>
+      <c r="P33" s="42"/>
+      <c r="Q33" s="19"/>
+    </row>
+    <row r="34" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C34" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="D33" s="32" t="s">
+      <c r="D34" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="E33" s="32">
+      <c r="E34" s="25">
         <v>2.5</v>
       </c>
-      <c r="F33" s="46"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="23"/>
-      <c r="J33" s="25"/>
-      <c r="K33" s="25"/>
-      <c r="L33" s="23"/>
-      <c r="M33" s="23"/>
-      <c r="N33" s="23"/>
-      <c r="O33" s="23"/>
-      <c r="P33" s="23"/>
-    </row>
-    <row r="34" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C34" s="32" t="s">
+      <c r="F34" s="2"/>
+      <c r="G34" s="45">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="H34" s="17"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="21"/>
+      <c r="L34" s="21"/>
+      <c r="M34" s="19"/>
+      <c r="N34" s="19"/>
+      <c r="O34" s="19"/>
+      <c r="P34" s="19"/>
+      <c r="Q34" s="19"/>
+    </row>
+    <row r="35" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C35" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="D34" s="32" t="s">
+      <c r="D35" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E34" s="32">
+      <c r="E35" s="25">
         <v>15</v>
       </c>
-      <c r="F34" s="46"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="23"/>
-      <c r="I34" s="23"/>
-      <c r="J34" s="25"/>
-      <c r="K34" s="25"/>
-      <c r="L34" s="28"/>
-      <c r="M34" s="28"/>
-      <c r="N34" s="28"/>
-      <c r="O34" s="23"/>
-      <c r="P34" s="23"/>
-    </row>
-    <row r="35" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C35" s="32" t="s">
+      <c r="F35" s="2"/>
+      <c r="G35" s="45">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="H35" s="17"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="21"/>
+      <c r="L35" s="21"/>
+      <c r="M35" s="32"/>
+      <c r="N35" s="12"/>
+      <c r="O35" s="29"/>
+      <c r="P35" s="19"/>
+      <c r="Q35" s="19"/>
+    </row>
+    <row r="36" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C36" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="D35" s="32" t="s">
+      <c r="D36" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="E35" s="32">
+      <c r="E36" s="25">
         <v>3</v>
       </c>
-      <c r="F35" s="47">
+      <c r="F36" s="41">
         <v>1</v>
       </c>
-      <c r="G35" s="21"/>
-      <c r="H35" s="23"/>
-      <c r="I35" s="23"/>
-      <c r="J35" s="25"/>
-      <c r="K35" s="25"/>
-      <c r="L35" s="23"/>
-      <c r="M35" s="23"/>
-      <c r="N35" s="23"/>
-      <c r="O35" s="23"/>
-      <c r="P35" s="23"/>
-    </row>
-    <row r="36" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C36" s="32" t="s">
+      <c r="G36" s="47">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H36" s="38"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="21"/>
+      <c r="L36" s="21"/>
+      <c r="M36" s="19"/>
+      <c r="N36" s="19"/>
+      <c r="O36" s="19"/>
+      <c r="P36" s="19"/>
+      <c r="Q36" s="19"/>
+    </row>
+    <row r="37" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C37" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="D36" s="37" t="s">
+      <c r="D37" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="E36" s="36">
+      <c r="E37" s="29">
         <v>2</v>
       </c>
-      <c r="F36" s="47">
+      <c r="F37" s="20">
         <v>1</v>
       </c>
-      <c r="G36" s="21"/>
-      <c r="H36" s="23"/>
-      <c r="I36" s="23"/>
-      <c r="J36" s="25"/>
-      <c r="K36" s="25"/>
-      <c r="L36" s="23"/>
-      <c r="M36" s="23"/>
-      <c r="N36" s="23"/>
-      <c r="O36" s="23"/>
-      <c r="P36" s="23"/>
-    </row>
-    <row r="37" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C37" s="32" t="s">
+      <c r="G37" s="47">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H37" s="38"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="21"/>
+      <c r="L37" s="21"/>
+      <c r="M37" s="19"/>
+      <c r="N37" s="19"/>
+      <c r="O37" s="19"/>
+      <c r="P37" s="19"/>
+      <c r="Q37" s="19"/>
+    </row>
+    <row r="38" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C38" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="D37" s="37" t="s">
+      <c r="D38" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="E37" s="36">
+      <c r="E38" s="29">
         <v>1</v>
       </c>
-      <c r="F37" s="47">
+      <c r="F38" s="20">
         <v>3</v>
       </c>
-      <c r="G37" s="21"/>
-      <c r="H37" s="23"/>
-      <c r="I37" s="23"/>
-      <c r="J37" s="25"/>
-      <c r="K37" s="25"/>
-      <c r="L37" s="23"/>
-      <c r="M37" s="23"/>
-      <c r="N37" s="23"/>
-      <c r="O37" s="23"/>
-      <c r="P37" s="23"/>
-    </row>
-    <row r="38" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C38" s="32" t="s">
+      <c r="G38" s="47">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="H38" s="38"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="19"/>
+      <c r="K38" s="21"/>
+      <c r="L38" s="21"/>
+      <c r="M38" s="19"/>
+      <c r="N38" s="19"/>
+      <c r="O38" s="19"/>
+      <c r="P38" s="19"/>
+      <c r="Q38" s="19"/>
+    </row>
+    <row r="39" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C39" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="D38" s="32" t="s">
+      <c r="D39" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="E38" s="32">
+      <c r="E39" s="25">
         <v>1</v>
       </c>
-      <c r="F38" s="48"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="24"/>
-      <c r="I38" s="23"/>
-      <c r="J38" s="25"/>
-      <c r="K38" s="25"/>
-      <c r="L38" s="23"/>
-      <c r="M38" s="23"/>
-      <c r="N38" s="23"/>
-      <c r="O38" s="23"/>
-      <c r="P38" s="23"/>
-    </row>
-    <row r="39" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C39" s="32" t="s">
+      <c r="F39" s="3"/>
+      <c r="G39" s="45">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H39" s="18"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="21"/>
+      <c r="L39" s="21"/>
+      <c r="M39" s="19"/>
+      <c r="N39" s="19"/>
+      <c r="O39" s="19"/>
+      <c r="P39" s="19"/>
+      <c r="Q39" s="19"/>
+    </row>
+    <row r="40" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C40" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="D39" s="32" t="s">
+      <c r="D40" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E39" s="32">
+      <c r="E40" s="25">
         <v>2</v>
       </c>
-      <c r="F39" s="48"/>
-      <c r="G39" s="22"/>
-      <c r="H39" s="28"/>
-      <c r="I39" s="23"/>
-      <c r="J39" s="25"/>
-      <c r="K39" s="25"/>
-      <c r="L39" s="23"/>
-      <c r="M39" s="23"/>
-      <c r="N39" s="23"/>
-      <c r="O39" s="23"/>
-      <c r="P39" s="23"/>
-    </row>
-    <row r="40" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C40" s="32" t="s">
+      <c r="F40" s="41">
+        <v>3</v>
+      </c>
+      <c r="G40" s="45">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="H40" s="18"/>
+      <c r="I40" s="11"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="21"/>
+      <c r="L40" s="21"/>
+      <c r="M40" s="19"/>
+      <c r="N40" s="19"/>
+      <c r="O40" s="19"/>
+      <c r="P40" s="19"/>
+      <c r="Q40" s="19"/>
+    </row>
+    <row r="41" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C41" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="D40" s="18" t="s">
+      <c r="D41" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="E40" s="18">
+      <c r="E41" s="15">
         <v>1</v>
       </c>
-      <c r="F40" s="44"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="29"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="9"/>
-      <c r="K40" s="9"/>
-      <c r="L40" s="1"/>
-      <c r="M40" s="1"/>
-      <c r="N40" s="1"/>
-      <c r="O40" s="1"/>
-      <c r="P40" s="1"/>
-    </row>
-    <row r="41" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C41" s="32"/>
-      <c r="D41" s="33"/>
-      <c r="E41" s="33">
-        <f>SUM(E31:E40)</f>
-        <v>41</v>
-      </c>
-      <c r="F41" s="49">
-        <f>SUM(F31:F39)</f>
-        <v>5</v>
-      </c>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="9"/>
-      <c r="K41" s="9"/>
-      <c r="L41" s="1"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="45">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H41" s="17"/>
+      <c r="I41" s="39"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="8"/>
+      <c r="L41" s="8"/>
       <c r="M41" s="1"/>
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
-    </row>
-    <row r="42" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C42" s="32" t="s">
+      <c r="Q41" s="1"/>
+    </row>
+    <row r="42" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C42" s="25"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26">
+        <f>SUM(E32:E41)</f>
+        <v>41</v>
+      </c>
+      <c r="F42" s="26">
+        <f>SUM(F32:F40)</f>
+        <v>8</v>
+      </c>
+      <c r="G42" s="46">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="H42" s="17"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="8"/>
+      <c r="L42" s="8"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1"/>
+      <c r="O42" s="1"/>
+      <c r="P42" s="1"/>
+      <c r="Q42" s="1"/>
+    </row>
+    <row r="43" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C43" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="D42" s="35" t="s">
+      <c r="D43" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="E42" s="35">
+      <c r="E43" s="28">
+        <v>3</v>
+      </c>
+      <c r="F43" s="25"/>
+      <c r="G43" s="45">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>

</xml_diff>